<commit_message>
Fixed bugs and updated README file on installation process.
</commit_message>
<xml_diff>
--- a/demos/public_good_experiment/public_good_experiment_prompt_template.xlsx
+++ b/demos/public_good_experiment/public_good_experiment_prompt_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlow/Documents/talking-to-machines/talking-to-machines/demos/public_good_experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8160527-915F-B148-B539-C89068531890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9672724-2862-8848-9024-BD3AD8B23135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="-20740" windowWidth="30760" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5800" yWindow="-20740" windowWidth="30760" windowHeight="20140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_setting" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="129">
   <si>
     <t>experimental_setting</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Are you a republican?</t>
-  </si>
-  <si>
-    <t>public_question</t>
   </si>
   <si>
     <t xml:space="preserve">General Overview
@@ -809,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -822,7 +819,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1"/>
     </row>
@@ -836,7 +833,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -1942,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -3010,10 +3007,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4055,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M852"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4133,10 +4130,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>29</v>
@@ -4163,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -4172,19 +4169,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" s="3" t="b">
         <v>1</v>
@@ -4204,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -4213,19 +4210,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J4" s="3" t="b">
         <v>1</v>
@@ -4245,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -4254,19 +4251,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="3" t="b">
         <v>1</v>
@@ -4295,19 +4292,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J6" s="3" t="b">
         <v>0</v>
@@ -4336,19 +4333,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7" s="3" t="b">
         <v>0</v>
@@ -4377,19 +4374,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J8" s="3" t="b">
         <v>0</v>
@@ -4418,19 +4415,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J9" s="3" t="b">
         <v>0</v>
@@ -4459,19 +4456,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="I10" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10" s="3" t="b">
         <v>0</v>

</xml_diff>